<commit_message>
revisi kk dan inventarisasi
</commit_message>
<xml_diff>
--- a/report/template/PEROLEHAN/revisi-template_kk_v4.xlsx
+++ b/report/template/PEROLEHAN/revisi-template_kk_v4.xlsx
@@ -83,10 +83,10 @@
     <t xml:space="preserve">MUTASI TAMBAH</t>
   </si>
   <si>
-    <t xml:space="preserve">MUTASI KURANG</t>
+    <t xml:space="preserve">BEBAN PENYUSUTAN TAHUN BERJALAN</t>
   </si>
   <si>
-    <t xml:space="preserve">BEBAN PENYUSUTAN TAHUN BERJALAN</t>
+    <t xml:space="preserve">MUTASI KURANG</t>
   </si>
   <si>
     <t xml:space="preserve">SALDO AKHIR</t>
@@ -312,6 +312,9 @@
     <t xml:space="preserve">[a.bp_penyusutan_tambah;block=tbs:row;ope=tbs:num]</t>
   </si>
   <si>
+    <t xml:space="preserve">[a.bp_berjalan;block=tbs:row;ope=tbs:num]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[a.koreksi_kurang_jml;block=tbs:row;ope=tbs:num]</t>
   </si>
   <si>
@@ -367,9 +370,6 @@
   </si>
   <si>
     <t xml:space="preserve">[a.bp_penyusutan_kurang;block=tbs:row;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[a.bp_berjalan;block=tbs:row;ope=tbs:num]</t>
   </si>
   <si>
     <t xml:space="preserve">[a.Saldo_akhir_jml;block=tbs:row;ope=tbs:num]</t>
@@ -843,6 +843,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -864,10 +868,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -970,9 +970,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>164520</xdr:colOff>
+      <xdr:colOff>164160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>145080</xdr:rowOff>
+      <xdr:rowOff>144720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -986,7 +986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="133560" y="0"/>
-          <a:ext cx="525960" cy="716400"/>
+          <a:ext cx="525600" cy="716040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1008,50 +1008,51 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="35" min="33" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="40" min="37" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="48" min="44" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="54" min="52" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="2" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="59" min="57" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="1" width="44.4132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="61" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="35" min="33" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="41" min="38" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="49" min="45" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="55" min="53" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="2" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="59" min="57" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="1" width="43.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1023" min="61" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1091,7 @@
       <c r="AG1" s="0"/>
       <c r="AH1" s="0"/>
       <c r="AI1" s="0"/>
-      <c r="AJ1" s="0"/>
+      <c r="AJ1" s="3"/>
       <c r="AK1" s="0"/>
       <c r="AL1" s="0"/>
       <c r="AM1" s="0"/>
@@ -1109,7 +1110,7 @@
       <c r="AZ1" s="0"/>
       <c r="BA1" s="0"/>
       <c r="BB1" s="0"/>
-      <c r="BC1" s="3"/>
+      <c r="BC1" s="0"/>
       <c r="BD1" s="0"/>
       <c r="BE1" s="0"/>
       <c r="BF1" s="0"/>
@@ -2078,7 +2079,6 @@
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -2118,7 +2118,7 @@
       <c r="AG2" s="0"/>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
-      <c r="AJ2" s="0"/>
+      <c r="AJ2" s="3"/>
       <c r="AK2" s="0"/>
       <c r="AL2" s="0"/>
       <c r="AM2" s="0"/>
@@ -2137,7 +2137,7 @@
       <c r="AZ2" s="0"/>
       <c r="BA2" s="0"/>
       <c r="BB2" s="0"/>
-      <c r="BC2" s="3"/>
+      <c r="BC2" s="0"/>
       <c r="BD2" s="0"/>
       <c r="BE2" s="0"/>
       <c r="BF2" s="0"/>
@@ -3106,7 +3106,6 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -3146,7 +3145,7 @@
       <c r="AG3" s="0"/>
       <c r="AH3" s="0"/>
       <c r="AI3" s="0"/>
-      <c r="AJ3" s="0"/>
+      <c r="AJ3" s="3"/>
       <c r="AK3" s="0"/>
       <c r="AL3" s="0"/>
       <c r="AM3" s="0"/>
@@ -3165,7 +3164,7 @@
       <c r="AZ3" s="0"/>
       <c r="BA3" s="0"/>
       <c r="BB3" s="0"/>
-      <c r="BC3" s="3"/>
+      <c r="BC3" s="0"/>
       <c r="BD3" s="0"/>
       <c r="BE3" s="0"/>
       <c r="BF3" s="0"/>
@@ -4134,7 +4133,6 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -4172,7 +4170,7 @@
       <c r="AG4" s="0"/>
       <c r="AH4" s="0"/>
       <c r="AI4" s="0"/>
-      <c r="AJ4" s="0"/>
+      <c r="AJ4" s="3"/>
       <c r="AK4" s="0"/>
       <c r="AL4" s="0"/>
       <c r="AM4" s="0"/>
@@ -4191,7 +4189,7 @@
       <c r="AZ4" s="0"/>
       <c r="BA4" s="0"/>
       <c r="BB4" s="0"/>
-      <c r="BC4" s="3"/>
+      <c r="BC4" s="0"/>
       <c r="BD4" s="0"/>
       <c r="BE4" s="0"/>
       <c r="BF4" s="0"/>
@@ -5160,7 +5158,6 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -5198,7 +5195,7 @@
       <c r="AG5" s="0"/>
       <c r="AH5" s="0"/>
       <c r="AI5" s="0"/>
-      <c r="AJ5" s="0"/>
+      <c r="AJ5" s="3"/>
       <c r="AK5" s="0"/>
       <c r="AL5" s="0"/>
       <c r="AM5" s="0"/>
@@ -5217,7 +5214,7 @@
       <c r="AZ5" s="0"/>
       <c r="BA5" s="0"/>
       <c r="BB5" s="0"/>
-      <c r="BC5" s="3"/>
+      <c r="BC5" s="0"/>
       <c r="BD5" s="0"/>
       <c r="BE5" s="0"/>
       <c r="BF5" s="0"/>
@@ -6186,7 +6183,6 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
@@ -6228,7 +6224,7 @@
       <c r="AG6" s="0"/>
       <c r="AH6" s="0"/>
       <c r="AI6" s="0"/>
-      <c r="AJ6" s="0"/>
+      <c r="AJ6" s="3"/>
       <c r="AK6" s="0"/>
       <c r="AL6" s="0"/>
       <c r="AM6" s="0"/>
@@ -6247,7 +6243,7 @@
       <c r="AZ6" s="0"/>
       <c r="BA6" s="0"/>
       <c r="BB6" s="0"/>
-      <c r="BC6" s="3"/>
+      <c r="BC6" s="0"/>
       <c r="BD6" s="0"/>
       <c r="BE6" s="0"/>
       <c r="BF6" s="0"/>
@@ -7216,7 +7212,6 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
@@ -7258,7 +7253,7 @@
       <c r="AG7" s="0"/>
       <c r="AH7" s="0"/>
       <c r="AI7" s="0"/>
-      <c r="AJ7" s="0"/>
+      <c r="AJ7" s="3"/>
       <c r="AK7" s="0"/>
       <c r="AL7" s="0"/>
       <c r="AM7" s="0"/>
@@ -7277,7 +7272,7 @@
       <c r="AZ7" s="0"/>
       <c r="BA7" s="0"/>
       <c r="BB7" s="0"/>
-      <c r="BC7" s="3"/>
+      <c r="BC7" s="0"/>
       <c r="BD7" s="0"/>
       <c r="BE7" s="0"/>
       <c r="BF7" s="0"/>
@@ -8246,7 +8241,6 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
@@ -8288,7 +8282,7 @@
       <c r="AG8" s="0"/>
       <c r="AH8" s="0"/>
       <c r="AI8" s="0"/>
-      <c r="AJ8" s="0"/>
+      <c r="AJ8" s="3"/>
       <c r="AK8" s="0"/>
       <c r="AL8" s="0"/>
       <c r="AM8" s="0"/>
@@ -8307,7 +8301,7 @@
       <c r="AZ8" s="0"/>
       <c r="BA8" s="0"/>
       <c r="BB8" s="0"/>
-      <c r="BC8" s="3"/>
+      <c r="BC8" s="0"/>
       <c r="BD8" s="0"/>
       <c r="BE8" s="0"/>
       <c r="BF8" s="0"/>
@@ -9276,7 +9270,6 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
@@ -9318,7 +9311,7 @@
       <c r="AG9" s="0"/>
       <c r="AH9" s="0"/>
       <c r="AI9" s="0"/>
-      <c r="AJ9" s="0"/>
+      <c r="AJ9" s="3"/>
       <c r="AK9" s="0"/>
       <c r="AL9" s="0"/>
       <c r="AM9" s="0"/>
@@ -9337,7 +9330,7 @@
       <c r="AZ9" s="0"/>
       <c r="BA9" s="0"/>
       <c r="BB9" s="0"/>
-      <c r="BC9" s="3"/>
+      <c r="BC9" s="0"/>
       <c r="BD9" s="0"/>
       <c r="BE9" s="0"/>
       <c r="BF9" s="0"/>
@@ -10306,7 +10299,6 @@
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
@@ -10348,7 +10340,7 @@
       <c r="AG10" s="0"/>
       <c r="AH10" s="0"/>
       <c r="AI10" s="0"/>
-      <c r="AJ10" s="0"/>
+      <c r="AJ10" s="3"/>
       <c r="AK10" s="0"/>
       <c r="AL10" s="0"/>
       <c r="AM10" s="0"/>
@@ -10367,7 +10359,7 @@
       <c r="AZ10" s="0"/>
       <c r="BA10" s="0"/>
       <c r="BB10" s="0"/>
-      <c r="BC10" s="3"/>
+      <c r="BC10" s="0"/>
       <c r="BD10" s="0"/>
       <c r="BE10" s="0"/>
       <c r="BF10" s="0"/>
@@ -11336,7 +11328,6 @@
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
@@ -11378,7 +11369,7 @@
       <c r="AG11" s="0"/>
       <c r="AH11" s="0"/>
       <c r="AI11" s="0"/>
-      <c r="AJ11" s="0"/>
+      <c r="AJ11" s="3"/>
       <c r="AK11" s="0"/>
       <c r="AL11" s="0"/>
       <c r="AM11" s="0"/>
@@ -11397,7 +11388,7 @@
       <c r="AZ11" s="0"/>
       <c r="BA11" s="0"/>
       <c r="BB11" s="0"/>
-      <c r="BC11" s="3"/>
+      <c r="BC11" s="0"/>
       <c r="BD11" s="0"/>
       <c r="BE11" s="0"/>
       <c r="BF11" s="0"/>
@@ -12366,7 +12357,6 @@
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
@@ -12404,7 +12394,7 @@
       <c r="AG12" s="0"/>
       <c r="AH12" s="0"/>
       <c r="AI12" s="0"/>
-      <c r="AJ12" s="0"/>
+      <c r="AJ12" s="3"/>
       <c r="AK12" s="0"/>
       <c r="AL12" s="0"/>
       <c r="AM12" s="0"/>
@@ -12423,7 +12413,7 @@
       <c r="AZ12" s="0"/>
       <c r="BA12" s="0"/>
       <c r="BB12" s="0"/>
-      <c r="BC12" s="3"/>
+      <c r="BC12" s="0"/>
       <c r="BD12" s="0"/>
       <c r="BE12" s="0"/>
       <c r="BF12" s="0"/>
@@ -13392,7 +13382,6 @@
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="15" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
@@ -13442,10 +13431,12 @@
       <c r="AG13" s="11"/>
       <c r="AH13" s="11"/>
       <c r="AI13" s="11"/>
-      <c r="AJ13" s="11" t="s">
+      <c r="AJ13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AK13" s="11"/>
+      <c r="AK13" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="AL13" s="11"/>
       <c r="AM13" s="11"/>
       <c r="AN13" s="11"/>
@@ -13463,9 +13454,7 @@
       <c r="AZ13" s="11"/>
       <c r="BA13" s="11"/>
       <c r="BB13" s="11"/>
-      <c r="BC13" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="BC13" s="11"/>
       <c r="BD13" s="13" t="s">
         <v>22</v>
       </c>
@@ -13475,6 +13464,7 @@
       <c r="BH13" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
@@ -13532,40 +13522,40 @@
       <c r="AI14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AJ14" s="21" t="s">
+      <c r="AJ14" s="12"/>
+      <c r="AK14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="AK14" s="21"/>
-      <c r="AL14" s="22" t="s">
+      <c r="AL14" s="21"/>
+      <c r="AM14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AM14" s="22"/>
       <c r="AN14" s="22"/>
       <c r="AO14" s="22"/>
       <c r="AP14" s="22"/>
-      <c r="AQ14" s="16" t="s">
+      <c r="AQ14" s="22"/>
+      <c r="AR14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AR14" s="16"/>
-      <c r="AS14" s="23" t="s">
+      <c r="AS14" s="16"/>
+      <c r="AT14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AT14" s="23"/>
       <c r="AU14" s="23"/>
       <c r="AV14" s="23"/>
       <c r="AW14" s="23"/>
       <c r="AX14" s="23"/>
-      <c r="AY14" s="24" t="s">
+      <c r="AY14" s="23"/>
+      <c r="AZ14" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AZ14" s="24"/>
-      <c r="BA14" s="25" t="s">
+      <c r="BA14" s="24"/>
+      <c r="BB14" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BB14" s="25" t="s">
+      <c r="BC14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BC14" s="12"/>
       <c r="BD14" s="13"/>
       <c r="BE14" s="13"/>
       <c r="BF14" s="13"/>
@@ -14534,7 +14524,6 @@
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
@@ -14590,44 +14579,44 @@
       <c r="AG15" s="19"/>
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
-      <c r="AJ15" s="21"/>
+      <c r="AJ15" s="12"/>
       <c r="AK15" s="21"/>
-      <c r="AL15" s="28" t="s">
+      <c r="AL15" s="21"/>
+      <c r="AM15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="AM15" s="28" t="s">
+      <c r="AN15" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="AN15" s="28" t="s">
+      <c r="AO15" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="AO15" s="29" t="s">
+      <c r="AP15" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AP15" s="29"/>
-      <c r="AQ15" s="16"/>
+      <c r="AQ15" s="29"/>
       <c r="AR15" s="16"/>
-      <c r="AS15" s="23" t="s">
+      <c r="AS15" s="16"/>
+      <c r="AT15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AT15" s="23" t="s">
+      <c r="AU15" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AU15" s="23" t="s">
+      <c r="AV15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AV15" s="23" t="s">
+      <c r="AW15" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AW15" s="29" t="s">
+      <c r="AX15" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AX15" s="29"/>
-      <c r="AY15" s="24"/>
+      <c r="AY15" s="29"/>
       <c r="AZ15" s="24"/>
-      <c r="BA15" s="25"/>
+      <c r="BA15" s="24"/>
       <c r="BB15" s="25"/>
-      <c r="BC15" s="12"/>
+      <c r="BC15" s="25"/>
       <c r="BD15" s="13" t="s">
         <v>40</v>
       </c>
@@ -15602,7 +15591,6 @@
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
@@ -15692,48 +15680,48 @@
       <c r="AI16" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AJ16" s="21" t="s">
+      <c r="AJ16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AK16" s="32" t="s">
+      <c r="AL16" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="AL16" s="33"/>
       <c r="AM16" s="33"/>
       <c r="AN16" s="33"/>
-      <c r="AO16" s="29" t="s">
+      <c r="AO16" s="33"/>
+      <c r="AP16" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="AP16" s="22" t="s">
+      <c r="AQ16" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AQ16" s="16" t="s">
+      <c r="AR16" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="AR16" s="23" t="s">
+      <c r="AS16" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="AS16" s="33"/>
       <c r="AT16" s="33"/>
       <c r="AU16" s="33"/>
       <c r="AV16" s="33"/>
-      <c r="AW16" s="29" t="s">
+      <c r="AW16" s="33"/>
+      <c r="AX16" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="AX16" s="22" t="s">
+      <c r="AY16" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AY16" s="24" t="s">
+      <c r="AZ16" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AZ16" s="25" t="s">
+      <c r="BA16" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="BA16" s="25"/>
-      <c r="BB16" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC16" s="12" t="s">
+      <c r="BB16" s="25"/>
+      <c r="BC16" s="25" t="s">
         <v>58</v>
       </c>
       <c r="BD16" s="13" t="s">
@@ -16712,7 +16700,6 @@
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="42" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="34" t="n">
@@ -16728,99 +16715,104 @@
       <c r="G17" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="H17" s="34"/>
+      <c r="H17" s="34" t="n">
+        <v>4</v>
+      </c>
       <c r="I17" s="34"/>
       <c r="J17" s="35" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
       <c r="N17" s="34" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O17" s="34"/>
       <c r="P17" s="34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
       <c r="T17" s="34" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U17" s="34"/>
       <c r="V17" s="34"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="Z17" s="34" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC17" s="34"/>
       <c r="AD17" s="34" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AE17" s="34"/>
       <c r="AF17" s="36" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AG17" s="36"/>
       <c r="AH17" s="37" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AI17" s="37" t="n">
-        <v>14</v>
-      </c>
-      <c r="AJ17" s="38" t="n">
         <v>15</v>
       </c>
-      <c r="AK17" s="38"/>
-      <c r="AL17" s="34" t="n">
+      <c r="AJ17" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="AM17" s="34"/>
+      <c r="AK17" s="38" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL17" s="38"/>
+      <c r="AM17" s="34" t="n">
+        <v>18</v>
+      </c>
       <c r="AN17" s="34"/>
       <c r="AO17" s="34"/>
       <c r="AP17" s="34"/>
-      <c r="AQ17" s="34" t="n">
-        <v>17</v>
-      </c>
-      <c r="AR17" s="34"/>
-      <c r="AS17" s="34" t="n">
-        <v>18</v>
-      </c>
-      <c r="AT17" s="34"/>
+      <c r="AQ17" s="34"/>
+      <c r="AR17" s="34" t="n">
+        <v>19</v>
+      </c>
+      <c r="AS17" s="34"/>
+      <c r="AT17" s="34" t="n">
+        <v>20</v>
+      </c>
       <c r="AU17" s="34"/>
       <c r="AV17" s="34"/>
       <c r="AW17" s="34"/>
       <c r="AX17" s="34"/>
-      <c r="AY17" s="39" t="n">
-        <v>19</v>
-      </c>
-      <c r="AZ17" s="39"/>
-      <c r="BA17" s="39" t="n">
-        <v>20</v>
-      </c>
+      <c r="AY17" s="34"/>
+      <c r="AZ17" s="39" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA17" s="39"/>
       <c r="BB17" s="39" t="n">
-        <v>21</v>
-      </c>
-      <c r="BC17" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="BC17" s="39" t="n">
+        <v>23</v>
+      </c>
       <c r="BD17" s="40" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BE17" s="40"/>
       <c r="BF17" s="40"/>
       <c r="BG17" s="40"/>
       <c r="BH17" s="41" t="n">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="34"/>
@@ -16858,26 +16850,26 @@
       <c r="AG18" s="36"/>
       <c r="AH18" s="36"/>
       <c r="AI18" s="36"/>
-      <c r="AJ18" s="38"/>
+      <c r="AJ18" s="12"/>
       <c r="AK18" s="38"/>
-      <c r="AL18" s="34"/>
+      <c r="AL18" s="38"/>
       <c r="AM18" s="34"/>
       <c r="AN18" s="34"/>
-      <c r="AO18" s="49"/>
+      <c r="AO18" s="34"/>
       <c r="AP18" s="49"/>
-      <c r="AQ18" s="34"/>
+      <c r="AQ18" s="49"/>
       <c r="AR18" s="34"/>
       <c r="AS18" s="34"/>
       <c r="AT18" s="34"/>
       <c r="AU18" s="34"/>
       <c r="AV18" s="34"/>
-      <c r="AW18" s="49"/>
+      <c r="AW18" s="34"/>
       <c r="AX18" s="49"/>
-      <c r="AY18" s="39"/>
+      <c r="AY18" s="49"/>
       <c r="AZ18" s="39"/>
       <c r="BA18" s="39"/>
       <c r="BB18" s="39"/>
-      <c r="BC18" s="12"/>
+      <c r="BC18" s="39"/>
       <c r="BD18" s="40"/>
       <c r="BE18" s="40"/>
       <c r="BF18" s="40"/>
@@ -17846,7 +17838,6 @@
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" s="76" customFormat="true" ht="16.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="51"/>
@@ -17958,7 +17949,7 @@
       <c r="AK19" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="AL19" s="53" t="s">
+      <c r="AL19" s="68" t="s">
         <v>96</v>
       </c>
       <c r="AM19" s="53" t="s">
@@ -17967,16 +17958,16 @@
       <c r="AN19" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="AO19" s="68" t="s">
+      <c r="AO19" s="53" t="s">
         <v>99</v>
       </c>
       <c r="AP19" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="AQ19" s="56" t="s">
+      <c r="AQ19" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="AR19" s="53" t="s">
+      <c r="AR19" s="56" t="s">
         <v>102</v>
       </c>
       <c r="AS19" s="53" t="s">
@@ -17991,7 +17982,7 @@
       <c r="AV19" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AW19" s="68" t="s">
+      <c r="AW19" s="53" t="s">
         <v>107</v>
       </c>
       <c r="AX19" s="69" t="s">
@@ -18003,10 +17994,10 @@
       <c r="AZ19" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="BA19" s="71" t="s">
+      <c r="BA19" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="BB19" s="71" t="s">
+      <c r="BB19" s="72" t="s">
         <v>112</v>
       </c>
       <c r="BC19" s="72" t="s">
@@ -18027,6 +18018,7 @@
       <c r="BH19" s="75" t="s">
         <v>118</v>
       </c>
+      <c r="AMJ19" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="56">
@@ -18042,8 +18034,8 @@
     <mergeCell ref="H13:I15"/>
     <mergeCell ref="J13:M14"/>
     <mergeCell ref="N13:AI13"/>
-    <mergeCell ref="AJ13:BB13"/>
-    <mergeCell ref="BC13:BC15"/>
+    <mergeCell ref="AJ13:AJ15"/>
+    <mergeCell ref="AK13:BC13"/>
     <mergeCell ref="BD13:BG14"/>
     <mergeCell ref="BH13:BH16"/>
     <mergeCell ref="N14:O15"/>
@@ -18056,18 +18048,18 @@
     <mergeCell ref="AF14:AG15"/>
     <mergeCell ref="AH14:AH15"/>
     <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="AJ14:AK15"/>
-    <mergeCell ref="AL14:AP14"/>
-    <mergeCell ref="AQ14:AR15"/>
-    <mergeCell ref="AS14:AX14"/>
-    <mergeCell ref="AY14:AZ15"/>
-    <mergeCell ref="BA14:BA15"/>
+    <mergeCell ref="AK14:AL15"/>
+    <mergeCell ref="AM14:AQ14"/>
+    <mergeCell ref="AR14:AS15"/>
+    <mergeCell ref="AT14:AY14"/>
+    <mergeCell ref="AZ14:BA15"/>
     <mergeCell ref="BB14:BB15"/>
+    <mergeCell ref="BC14:BC15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="R15:S15"/>
     <mergeCell ref="V15:W15"/>
-    <mergeCell ref="AO15:AP15"/>
-    <mergeCell ref="AW15:AX15"/>
+    <mergeCell ref="AP15:AQ15"/>
+    <mergeCell ref="AX15:AY15"/>
     <mergeCell ref="BD15:BE15"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="H17:I17"/>
@@ -18080,11 +18072,11 @@
     <mergeCell ref="AB17:AC17"/>
     <mergeCell ref="AD17:AE17"/>
     <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AJ17:AK17"/>
-    <mergeCell ref="AL17:AP17"/>
-    <mergeCell ref="AQ17:AR17"/>
-    <mergeCell ref="AS17:AX17"/>
-    <mergeCell ref="AY17:AZ17"/>
+    <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="AM17:AQ17"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AT17:AY17"/>
+    <mergeCell ref="AZ17:BA17"/>
     <mergeCell ref="BD17:BG17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>